<commit_message>
Adding data & run-mode in excel.
</commit_message>
<xml_diff>
--- a/resources/testdata/AgentTestCases.xlsx
+++ b/resources/testdata/AgentTestCases.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="1" r:id="rId1"/>
@@ -145,10 +145,10 @@
     <t>Verify fields of agent creation page</t>
   </si>
   <si>
-    <t>checkDuplicateUPN</t>
-  </si>
-  <si>
     <t>abc.com</t>
+  </si>
+  <si>
+    <t>checkUPN</t>
   </si>
 </sst>
 </file>
@@ -499,8 +499,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -544,7 +544,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B4" t="s">
         <v>41</v>
@@ -792,7 +792,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
@@ -822,7 +822,7 @@
         <v>19</v>
       </c>
       <c r="C2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Reseller add & refactoring old code
</commit_message>
<xml_diff>
--- a/resources/testdata/AgentTestCases.xlsx
+++ b/resources/testdata/AgentTestCases.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="1" r:id="rId1"/>
@@ -499,7 +499,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -563,7 +563,7 @@
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -679,8 +679,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -793,7 +793,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>